<commit_message>
Bætti við tímum í dagbók
git-svn-id: https://tgapc93.rhi.hi.is/svn/softdev/2013/hopur19@4938 5d233661-44a1-474e-bded-f455fa16cf90
</commit_message>
<xml_diff>
--- a/dagbokRagnheidar.xlsx
+++ b/dagbokRagnheidar.xlsx
@@ -483,7 +483,7 @@
   <dimension ref="B2:J53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -690,27 +690,36 @@
       <c r="G16">
         <v>0.5</v>
       </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
       <c r="J16" s="3">
         <f t="shared" ref="J16:J21" si="1">SUM(C16:I16)</f>
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="17" spans="2:10">
       <c r="B17" t="s">
         <v>11</v>
       </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
       <c r="J17" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:10">
       <c r="B18" t="s">
         <v>12</v>
       </c>
+      <c r="I18">
+        <v>2</v>
+      </c>
       <c r="J18" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="2:10">
@@ -743,10 +752,12 @@
         <v>2.5</v>
       </c>
       <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
+      <c r="I21" s="4">
+        <v>1.25</v>
+      </c>
       <c r="J21" s="4">
         <f t="shared" si="1"/>
-        <v>2.5</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="22" spans="2:10">
@@ -755,7 +766,7 @@
       </c>
       <c r="J22" s="3">
         <f>SUM(J16:J21)</f>
-        <v>3</v>
+        <v>8.25</v>
       </c>
     </row>
     <row r="24" spans="2:10">
@@ -1007,7 +1018,7 @@
       </c>
       <c r="D47" s="3">
         <f t="shared" ref="D47:D52" si="4">J6+J16+J26+J36</f>
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="48" spans="2:10">
@@ -1016,7 +1027,7 @@
       </c>
       <c r="D48" s="3">
         <f t="shared" si="4"/>
-        <v>4.6669999999999998</v>
+        <v>5.6669999999999998</v>
       </c>
     </row>
     <row r="49" spans="2:4">
@@ -1025,7 +1036,7 @@
       </c>
       <c r="D49" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="2:4">
@@ -1053,7 +1064,7 @@
       <c r="C52" s="4"/>
       <c r="D52" s="4">
         <f t="shared" si="4"/>
-        <v>2.5</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="53" spans="2:4">
@@ -1062,7 +1073,7 @@
       </c>
       <c r="D53" s="5">
         <f>SUM(D47:D52)</f>
-        <v>8.6669999999999998</v>
+        <v>13.917</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bætti við tímum í dagbók RBH
git-svn-id: https://tgapc93.rhi.hi.is/svn/softdev/2013/hopur19@5663 5d233661-44a1-474e-bded-f455fa16cf90
</commit_message>
<xml_diff>
--- a/dagbokRagnheidar.xlsx
+++ b/dagbokRagnheidar.xlsx
@@ -483,7 +483,7 @@
   <dimension ref="B2:J53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -688,14 +688,14 @@
         <v>10</v>
       </c>
       <c r="G16">
-        <v>0.5</v>
+        <v>0.66700000000000004</v>
       </c>
       <c r="I16">
         <v>1</v>
       </c>
       <c r="J16" s="3">
         <f t="shared" ref="J16:J21" si="1">SUM(C16:I16)</f>
-        <v>1.5</v>
+        <v>1.667</v>
       </c>
     </row>
     <row r="17" spans="2:10">
@@ -766,7 +766,7 @@
       </c>
       <c r="J22" s="3">
         <f>SUM(J16:J21)</f>
-        <v>8.25</v>
+        <v>8.4169999999999998</v>
       </c>
     </row>
     <row r="24" spans="2:10">
@@ -831,9 +831,12 @@
       <c r="B27" t="s">
         <v>11</v>
       </c>
+      <c r="C27">
+        <v>0.75</v>
+      </c>
       <c r="J27" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="28" spans="2:10">
@@ -867,7 +870,9 @@
       <c r="B31" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="4"/>
+      <c r="C31" s="4">
+        <v>0.25</v>
+      </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
@@ -876,7 +881,7 @@
       <c r="I31" s="4"/>
       <c r="J31" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="32" spans="2:10">
@@ -885,7 +890,7 @@
       </c>
       <c r="J32" s="3">
         <f>SUM(J26:J31)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="2:10">
@@ -1018,7 +1023,7 @@
       </c>
       <c r="D47" s="3">
         <f t="shared" ref="D47:D52" si="4">J6+J16+J26+J36</f>
-        <v>2.5</v>
+        <v>2.6669999999999998</v>
       </c>
     </row>
     <row r="48" spans="2:10">
@@ -1027,7 +1032,7 @@
       </c>
       <c r="D48" s="3">
         <f t="shared" si="4"/>
-        <v>5.6669999999999998</v>
+        <v>6.4169999999999998</v>
       </c>
     </row>
     <row r="49" spans="2:4">
@@ -1064,7 +1069,7 @@
       <c r="C52" s="4"/>
       <c r="D52" s="4">
         <f t="shared" si="4"/>
-        <v>3.75</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53" spans="2:4">
@@ -1073,7 +1078,7 @@
       </c>
       <c r="D53" s="5">
         <f>SUM(D47:D52)</f>
-        <v>13.917</v>
+        <v>15.084</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bætti við í dagbók Ragnheiðar
git-svn-id: https://tgapc93.rhi.hi.is/svn/softdev/2013/hopur19@6726 5d233661-44a1-474e-bded-f455fa16cf90
</commit_message>
<xml_diff>
--- a/dagbokRagnheidar.xlsx
+++ b/dagbokRagnheidar.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="14920" tabRatio="500"/>
+    <workbookView xWindow="11320" yWindow="560" windowWidth="14280" windowHeight="14920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -482,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1001,9 +1001,11 @@
         <v>15</v>
       </c>
       <c r="C41" s="4">
-        <v>1</v>
-      </c>
-      <c r="D41" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="D41" s="4">
+        <v>0.5</v>
+      </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
@@ -1011,7 +1013,7 @@
       <c r="I41" s="4"/>
       <c r="J41" s="4">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="42" spans="2:10">
@@ -1020,7 +1022,7 @@
       </c>
       <c r="J42" s="3">
         <f>SUM(J36:J41)</f>
-        <v>4</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="45" spans="2:10">
@@ -1080,7 +1082,7 @@
       <c r="C52" s="4"/>
       <c r="D52" s="4">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="53" spans="2:4">
@@ -1089,7 +1091,7 @@
       </c>
       <c r="D53" s="5">
         <f>SUM(D47:D52)</f>
-        <v>24.084</v>
+        <v>26.584</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dagbók tilbúin hálftíma fram í tímann og skýrsla tilbúin fyrir pdf
git-svn-id: https://tgapc93.rhi.hi.is/svn/softdev/2013/hopur19@8658 5d233661-44a1-474e-bded-f455fa16cf90
</commit_message>
<xml_diff>
--- a/dagbokRagnheidar.xlsx
+++ b/dagbokRagnheidar.xlsx
@@ -8,7 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="24">
   <si>
     <t>Nafn</t>
   </si>
@@ -92,19 +91,13 @@
   </si>
   <si>
     <t>rbh1@hi.is</t>
-  </si>
-  <si>
-    <t>Finnur Jónasson</t>
-  </si>
-  <si>
-    <t>fij2@hi.is</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -119,14 +112,6 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -136,7 +121,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -153,22 +138,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -205,11 +220,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" b="0" i="1" baseline="0"/>
-              <a:t> Björk Halld</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" b="0" i="1" baseline="0"/>
-              <a:t>órsdóttir</a:t>
+              <a:t> Björk Halldórsdóttir</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" b="0" i="1"/>
           </a:p>
@@ -274,137 +285,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15.5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
-        </c:dLbls>
-        <c:firstSliceAng val="0"/>
-        <c:holeSize val="50"/>
-      </c:doughnutChart>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" b="0" i="1"/>
-              <a:t>Finnur J</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" b="0" i="1"/>
-              <a:t>ónasson</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" b="0" i="1"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:doughnutChart>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Sheet1 (2)'!$B$47:$B$52</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Rannsóknir</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Kröfulýsing</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Hönnun</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Forritun</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Prófanir</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Frágangur</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sheet1 (2)'!$C$47:$C$52</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>12.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>12.5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.0</c:v>
+                  <c:v>17.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -459,43 +340,6 @@
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>781050</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -834,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J53"/>
+  <dimension ref="B2:L53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="L44" sqref="L44"/>
+      <selection activeCell="M47" sqref="M47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1253,7 +1097,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="2:10">
+    <row r="34" spans="2:12">
       <c r="B34" t="s">
         <v>19</v>
       </c>
@@ -1278,8 +1122,14 @@
       <c r="I34" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="2:10">
+      <c r="J34" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12">
       <c r="C35" s="2">
         <v>41316</v>
       </c>
@@ -1301,8 +1151,14 @@
       <c r="I35" s="2">
         <v>41322</v>
       </c>
-    </row>
-    <row r="36" spans="2:10">
+      <c r="J35" s="8">
+        <v>41323</v>
+      </c>
+      <c r="K35" s="2">
+        <v>41324</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12">
       <c r="B36" t="s">
         <v>10</v>
       </c>
@@ -1312,33 +1168,35 @@
       <c r="G36">
         <v>2</v>
       </c>
-      <c r="J36" s="3">
-        <f t="shared" ref="J36:J41" si="3">SUM(C36:I36)</f>
+      <c r="J36" s="7"/>
+      <c r="L36" s="3">
+        <f>SUM(C36:K36)</f>
         <v>3.75</v>
       </c>
     </row>
-    <row r="37" spans="2:10">
+    <row r="37" spans="2:12">
       <c r="B37" t="s">
         <v>11</v>
       </c>
-      <c r="I37">
+      <c r="J37" s="7">
         <v>2</v>
       </c>
-      <c r="J37" s="3">
-        <f t="shared" si="3"/>
+      <c r="L37" s="3">
+        <f>SUM(C37:K37)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="2:10">
+    <row r="38" spans="2:12">
       <c r="B38" t="s">
         <v>12</v>
       </c>
-      <c r="J38" s="3">
-        <f t="shared" si="3"/>
+      <c r="J38" s="7"/>
+      <c r="L38" s="3">
+        <f>SUM(C38:K38)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:10">
+    <row r="39" spans="2:12">
       <c r="B39" t="s">
         <v>13</v>
       </c>
@@ -1351,21 +1209,23 @@
       <c r="G39">
         <v>5</v>
       </c>
-      <c r="J39" s="3">
-        <f t="shared" si="3"/>
+      <c r="J39" s="7"/>
+      <c r="L39" s="3">
+        <f>SUM(C39:K39)</f>
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="2:10">
+    <row r="40" spans="2:12">
       <c r="B40" t="s">
         <v>14</v>
       </c>
-      <c r="J40" s="3">
-        <f t="shared" si="3"/>
+      <c r="J40" s="7"/>
+      <c r="L40" s="3">
+        <f>SUM(C40:K40)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:10" ht="16" thickBot="1">
+    <row r="41" spans="2:12" ht="16" thickBot="1">
       <c r="B41" s="4" t="s">
         <v>15</v>
       </c>
@@ -1383,43 +1243,47 @@
         <v>1.5</v>
       </c>
       <c r="H41" s="4"/>
-      <c r="I41" s="4">
+      <c r="I41" s="4"/>
+      <c r="J41" s="9">
         <v>5.5</v>
       </c>
-      <c r="J41" s="4">
-        <f t="shared" si="3"/>
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="42" spans="2:10">
+      <c r="K41" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="L41" s="4">
+        <f>SUM(C41:K41)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12">
       <c r="B42" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="J42" s="3">
-        <f>SUM(J36:J41)</f>
-        <v>28.25</v>
-      </c>
-    </row>
-    <row r="45" spans="2:10">
+      <c r="L42" s="3">
+        <f>SUM(L36:L41)</f>
+        <v>29.75</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12">
       <c r="B45" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="2:10">
+    <row r="47" spans="2:12">
       <c r="B47" t="s">
         <v>10</v>
       </c>
       <c r="C47" s="3">
-        <f>J6+J16+J26+J36</f>
+        <f>J6+J16+J26+L36</f>
         <v>8.4169999999999998</v>
       </c>
     </row>
-    <row r="48" spans="2:10">
+    <row r="48" spans="2:12">
       <c r="B48" t="s">
         <v>11</v>
       </c>
       <c r="C48" s="3">
-        <f>J7+J17+J27+J37</f>
+        <f>J7+J17+J27+L37</f>
         <v>8.4169999999999998</v>
       </c>
     </row>
@@ -1428,7 +1292,7 @@
         <v>12</v>
       </c>
       <c r="C49" s="3">
-        <f>J8+J18+J28+J38</f>
+        <f>J8+J18+J28+L38</f>
         <v>2</v>
       </c>
     </row>
@@ -1437,7 +1301,7 @@
         <v>13</v>
       </c>
       <c r="C50" s="3">
-        <f>J9+J19+J29+J39</f>
+        <f>J9+J19+J29+L39</f>
         <v>14</v>
       </c>
     </row>
@@ -1446,7 +1310,7 @@
         <v>14</v>
       </c>
       <c r="C51" s="3">
-        <f>J10+J20+J30+J40</f>
+        <f>J10+J20+J30+L40</f>
         <v>0</v>
       </c>
     </row>
@@ -1455,8 +1319,8 @@
         <v>15</v>
       </c>
       <c r="C52" s="4">
-        <f>J11+J21+J31+J41</f>
-        <v>15.5</v>
+        <f>J11+J21+J31+L41</f>
+        <v>17</v>
       </c>
     </row>
     <row r="53" spans="2:3">
@@ -1465,7 +1329,7 @@
       </c>
       <c r="C53" s="5">
         <f>SUM(C47:C52)</f>
-        <v>48.334000000000003</v>
+        <v>49.834000000000003</v>
       </c>
     </row>
   </sheetData>
@@ -1477,645 +1341,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J53"/>
-  <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="J43" sqref="J43"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="2" max="2" width="11.1640625" customWidth="1"/>
-    <col min="3" max="9" width="10.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:10">
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10">
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10">
-      <c r="C5" s="2">
-        <v>41295</v>
-      </c>
-      <c r="D5" s="2">
-        <v>41296</v>
-      </c>
-      <c r="E5" s="2">
-        <v>41297</v>
-      </c>
-      <c r="F5" s="2">
-        <v>41298</v>
-      </c>
-      <c r="G5" s="2">
-        <v>41299</v>
-      </c>
-      <c r="H5" s="2">
-        <v>41300</v>
-      </c>
-      <c r="I5" s="2">
-        <v>41301</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10">
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6">
-        <v>2</v>
-      </c>
-      <c r="J6" s="3">
-        <f t="shared" ref="J6:J11" si="0">SUM(C6:I6)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10">
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7">
-        <v>3</v>
-      </c>
-      <c r="H7">
-        <v>1.5</v>
-      </c>
-      <c r="J7" s="3">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10">
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="J8" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10">
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J9" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10">
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" ht="16" thickBot="1">
-      <c r="B11" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10">
-      <c r="B12" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J12" s="3">
-        <f>SUM(J6:J11)</f>
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10">
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" t="s">
-        <v>4</v>
-      </c>
-      <c r="E14" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" t="s">
-        <v>6</v>
-      </c>
-      <c r="G14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10">
-      <c r="C15" s="2">
-        <v>41302</v>
-      </c>
-      <c r="D15" s="2">
-        <v>41303</v>
-      </c>
-      <c r="E15" s="2">
-        <v>41304</v>
-      </c>
-      <c r="F15" s="2">
-        <v>41305</v>
-      </c>
-      <c r="G15" s="2">
-        <v>41306</v>
-      </c>
-      <c r="H15" s="2">
-        <v>41307</v>
-      </c>
-      <c r="I15" s="2">
-        <v>41308</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10">
-      <c r="B16" t="s">
-        <v>10</v>
-      </c>
-      <c r="J16" s="3">
-        <f t="shared" ref="J16:J21" si="1">SUM(C16:I16)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10">
-      <c r="B17" t="s">
-        <v>11</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="I17">
-        <v>4</v>
-      </c>
-      <c r="J17" s="3">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10">
-      <c r="B18" t="s">
-        <v>12</v>
-      </c>
-      <c r="G18">
-        <v>0.8</v>
-      </c>
-      <c r="J18" s="3">
-        <f t="shared" si="1"/>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10">
-      <c r="B19" t="s">
-        <v>13</v>
-      </c>
-      <c r="G19">
-        <v>0.5</v>
-      </c>
-      <c r="J19" s="3">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10">
-      <c r="B20" t="s">
-        <v>14</v>
-      </c>
-      <c r="J20" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" ht="16" thickBot="1">
-      <c r="B21" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="J21" s="4">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10">
-      <c r="B22" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J22" s="3">
-        <f>SUM(J16:J21)</f>
-        <v>6.8</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10">
-      <c r="B24" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" t="s">
-        <v>3</v>
-      </c>
-      <c r="D24" t="s">
-        <v>4</v>
-      </c>
-      <c r="E24" t="s">
-        <v>5</v>
-      </c>
-      <c r="F24" t="s">
-        <v>6</v>
-      </c>
-      <c r="G24" t="s">
-        <v>7</v>
-      </c>
-      <c r="H24" t="s">
-        <v>8</v>
-      </c>
-      <c r="I24" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10">
-      <c r="C25" s="2">
-        <v>41309</v>
-      </c>
-      <c r="D25" s="2">
-        <v>41310</v>
-      </c>
-      <c r="E25" s="2">
-        <v>41311</v>
-      </c>
-      <c r="F25" s="2">
-        <v>41312</v>
-      </c>
-      <c r="G25" s="2">
-        <v>41313</v>
-      </c>
-      <c r="H25" s="2">
-        <v>41314</v>
-      </c>
-      <c r="I25" s="2">
-        <v>41315</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10">
-      <c r="B26" t="s">
-        <v>10</v>
-      </c>
-      <c r="G26">
-        <v>1.5</v>
-      </c>
-      <c r="J26" s="3">
-        <f t="shared" ref="J26:J31" si="2">SUM(C26:I26)</f>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10">
-      <c r="B27" t="s">
-        <v>11</v>
-      </c>
-      <c r="J27" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10">
-      <c r="B28" t="s">
-        <v>12</v>
-      </c>
-      <c r="I28">
-        <v>0.5</v>
-      </c>
-      <c r="J28" s="3">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10">
-      <c r="B29" t="s">
-        <v>13</v>
-      </c>
-      <c r="I29">
-        <v>4</v>
-      </c>
-      <c r="J29" s="3">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10">
-      <c r="B30" t="s">
-        <v>14</v>
-      </c>
-      <c r="J30" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" ht="16" thickBot="1">
-      <c r="B31" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:10">
-      <c r="B32" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J32" s="3">
-        <f>SUM(J26:J31)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10">
-      <c r="B34" t="s">
-        <v>19</v>
-      </c>
-      <c r="C34" t="s">
-        <v>3</v>
-      </c>
-      <c r="D34" t="s">
-        <v>4</v>
-      </c>
-      <c r="E34" t="s">
-        <v>5</v>
-      </c>
-      <c r="F34" t="s">
-        <v>6</v>
-      </c>
-      <c r="G34" t="s">
-        <v>7</v>
-      </c>
-      <c r="H34" t="s">
-        <v>8</v>
-      </c>
-      <c r="I34" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="2:10">
-      <c r="C35" s="2">
-        <v>41316</v>
-      </c>
-      <c r="D35" s="2">
-        <v>41317</v>
-      </c>
-      <c r="E35" s="2">
-        <v>41318</v>
-      </c>
-      <c r="F35" s="2">
-        <v>41319</v>
-      </c>
-      <c r="G35" s="2">
-        <v>41320</v>
-      </c>
-      <c r="H35" s="2">
-        <v>41321</v>
-      </c>
-      <c r="I35" s="2">
-        <v>41322</v>
-      </c>
-    </row>
-    <row r="36" spans="2:10">
-      <c r="B36" t="s">
-        <v>10</v>
-      </c>
-      <c r="C36">
-        <v>0.5</v>
-      </c>
-      <c r="J36" s="3">
-        <f t="shared" ref="J36:J41" si="3">SUM(C36:I36)</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="37" spans="2:10">
-      <c r="B37" t="s">
-        <v>11</v>
-      </c>
-      <c r="C37">
-        <v>1</v>
-      </c>
-      <c r="F37">
-        <v>2</v>
-      </c>
-      <c r="J37" s="3">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="2:10">
-      <c r="B38" t="s">
-        <v>12</v>
-      </c>
-      <c r="F38">
-        <v>0.5</v>
-      </c>
-      <c r="J38" s="3">
-        <f t="shared" si="3"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="39" spans="2:10">
-      <c r="B39" t="s">
-        <v>13</v>
-      </c>
-      <c r="C39">
-        <v>3</v>
-      </c>
-      <c r="F39">
-        <v>5</v>
-      </c>
-      <c r="J39" s="3">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="2:10">
-      <c r="B40" t="s">
-        <v>14</v>
-      </c>
-      <c r="I40">
-        <v>3</v>
-      </c>
-      <c r="J40" s="3">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="2:10" ht="16" thickBot="1">
-      <c r="B41" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
-      <c r="H41" s="4"/>
-      <c r="I41" s="4">
-        <v>5.5</v>
-      </c>
-      <c r="J41" s="4">
-        <f t="shared" si="3"/>
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="42" spans="2:10">
-      <c r="B42" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J42" s="3">
-        <f>SUM(J36:J41)</f>
-        <v>20.5</v>
-      </c>
-    </row>
-    <row r="45" spans="2:10">
-      <c r="B45" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="47" spans="2:10">
-      <c r="B47" t="s">
-        <v>10</v>
-      </c>
-      <c r="C47" s="3">
-        <f>J6+J16+J26+J36</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="2:10">
-      <c r="B48" t="s">
-        <v>11</v>
-      </c>
-      <c r="C48" s="3">
-        <f>J7+J17+J27+J37</f>
-        <v>12.5</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3">
-      <c r="B49" t="s">
-        <v>12</v>
-      </c>
-      <c r="C49" s="3">
-        <f>J8+J18+J28+J38</f>
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3">
-      <c r="B50" t="s">
-        <v>13</v>
-      </c>
-      <c r="C50" s="3">
-        <f>J9+J19+J29+J39</f>
-        <v>12.5</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3">
-      <c r="B51" t="s">
-        <v>14</v>
-      </c>
-      <c r="C51" s="3">
-        <f>J10+J20+J30+J40</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3" ht="16" thickBot="1">
-      <c r="B52" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C52" s="4">
-        <f>J11+J21+J31+J41</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3">
-      <c r="B53" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C53" s="5">
-        <f>SUM(C47:C52)</f>
-        <v>39.799999999999997</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId2"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>